<commit_message>
[ CHECK FRAME ID BEFORE ADD SIGNAL ATTRIBUTES ]
</commit_message>
<xml_diff>
--- a/dbc/CAN_VARIANT/AnalyzeIds.xlsx
+++ b/dbc/CAN_VARIANT/AnalyzeIds.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="79">
   <si>
     <t>Result</t>
   </si>
@@ -168,6 +168,9 @@
   </si>
   <si>
     <t>0x706</t>
+  </si>
+  <si>
+    <t>STD</t>
   </si>
   <si>
     <t>intel</t>
@@ -799,7 +802,7 @@
         <v>46</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>42</v>
@@ -832,10 +835,10 @@
         <v>16</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X2" s="2" t="s">
         <v>42</v>
@@ -892,7 +895,7 @@
         <v>42</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:42">
@@ -909,7 +912,7 @@
         <v>43</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>42</v>
@@ -927,7 +930,7 @@
         <v>46</v>
       </c>
       <c r="K3" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L3" s="3" t="s">
         <v>42</v>
@@ -960,10 +963,10 @@
         <v>32</v>
       </c>
       <c r="V3" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W3" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X3" s="3" t="s">
         <v>42</v>
@@ -999,7 +1002,7 @@
         <v>1000</v>
       </c>
       <c r="AI3" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ3" s="3" t="s">
         <v>42</v>
@@ -1020,7 +1023,7 @@
         <v>42</v>
       </c>
       <c r="AP3" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:42">
@@ -1049,13 +1052,13 @@
         <v>42</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L4" s="2" t="s">
         <v>42</v>
@@ -1088,10 +1091,10 @@
         <v>16</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X4" s="2" t="s">
         <v>42</v>
@@ -1148,7 +1151,7 @@
         <v>42</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:42">
@@ -1165,25 +1168,25 @@
         <v>43</v>
       </c>
       <c r="E5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="K5" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>42</v>
@@ -1216,10 +1219,10 @@
         <v>32</v>
       </c>
       <c r="V5" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W5" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X5" s="3" t="s">
         <v>42</v>
@@ -1255,7 +1258,7 @@
         <v>1000</v>
       </c>
       <c r="AI5" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ5" s="3" t="s">
         <v>42</v>
@@ -1276,7 +1279,7 @@
         <v>42</v>
       </c>
       <c r="AP5" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:42">
@@ -1305,13 +1308,13 @@
         <v>42</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>42</v>
@@ -1344,10 +1347,10 @@
         <v>16</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>42</v>
@@ -1404,7 +1407,7 @@
         <v>42</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:42">
@@ -1421,25 +1424,25 @@
         <v>43</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>56</v>
-      </c>
       <c r="K7" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L7" s="3" t="s">
         <v>42</v>
@@ -1472,10 +1475,10 @@
         <v>32</v>
       </c>
       <c r="V7" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W7" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X7" s="3" t="s">
         <v>42</v>
@@ -1511,7 +1514,7 @@
         <v>1000</v>
       </c>
       <c r="AI7" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ7" s="3" t="s">
         <v>42</v>
@@ -1532,7 +1535,7 @@
         <v>42</v>
       </c>
       <c r="AP7" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:42">
@@ -1561,13 +1564,13 @@
         <v>42</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L8" s="2" t="s">
         <v>42</v>
@@ -1600,10 +1603,10 @@
         <v>16</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X8" s="2" t="s">
         <v>42</v>
@@ -1660,7 +1663,7 @@
         <v>42</v>
       </c>
       <c r="AP8" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:42">
@@ -1677,25 +1680,25 @@
         <v>43</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="J9" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="J9" s="3" t="s">
-        <v>59</v>
-      </c>
       <c r="K9" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L9" s="3" t="s">
         <v>42</v>
@@ -1728,10 +1731,10 @@
         <v>32</v>
       </c>
       <c r="V9" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W9" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X9" s="3" t="s">
         <v>42</v>
@@ -1767,7 +1770,7 @@
         <v>1000</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ9" s="3" t="s">
         <v>42</v>
@@ -1788,7 +1791,7 @@
         <v>42</v>
       </c>
       <c r="AP9" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:42">
@@ -1817,13 +1820,13 @@
         <v>42</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>42</v>
@@ -1856,10 +1859,10 @@
         <v>16</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>42</v>
@@ -1916,7 +1919,7 @@
         <v>42</v>
       </c>
       <c r="AP10" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:42">
@@ -1933,25 +1936,25 @@
         <v>43</v>
       </c>
       <c r="E11" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="J11" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="J11" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="K11" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L11" s="3" t="s">
         <v>42</v>
@@ -1984,10 +1987,10 @@
         <v>32</v>
       </c>
       <c r="V11" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W11" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X11" s="3" t="s">
         <v>42</v>
@@ -2023,7 +2026,7 @@
         <v>1000</v>
       </c>
       <c r="AI11" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ11" s="3" t="s">
         <v>42</v>
@@ -2044,7 +2047,7 @@
         <v>42</v>
       </c>
       <c r="AP11" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="12" spans="1:42">
@@ -2073,13 +2076,13 @@
         <v>42</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L12" s="2" t="s">
         <v>42</v>
@@ -2112,10 +2115,10 @@
         <v>16</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X12" s="2" t="s">
         <v>42</v>
@@ -2172,7 +2175,7 @@
         <v>42</v>
       </c>
       <c r="AP12" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:42">
@@ -2189,25 +2192,25 @@
         <v>43</v>
       </c>
       <c r="E13" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="K13" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="L13" s="3" t="s">
         <v>42</v>
@@ -2240,10 +2243,10 @@
         <v>32</v>
       </c>
       <c r="V13" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="W13" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="X13" s="3" t="s">
         <v>42</v>
@@ -2279,7 +2282,7 @@
         <v>1000</v>
       </c>
       <c r="AI13" s="3" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="AJ13" s="3" t="s">
         <v>42</v>
@@ -2300,7 +2303,7 @@
         <v>42</v>
       </c>
       <c r="AP13" s="3" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>
@@ -2319,22 +2322,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -2352,19 +2355,19 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>